<commit_message>
aanpassing schema en pcb
oplossing voor audiosignalen
in excel nog enkele links toegevoegd
</commit_message>
<xml_diff>
--- a/Bluetooth music box/schema's en pcb/schema_v1/BOM.xlsx
+++ b/Bluetooth music box/schema's en pcb/schema_v1/BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="170">
   <si>
     <t>Ref</t>
   </si>
@@ -221,9 +221,6 @@
     <t>Speaker</t>
   </si>
   <si>
-    <t>R1, R4, R6, R7, R11, R13, R16, R20, R22, R28, R32, R37</t>
-  </si>
-  <si>
     <t>10k</t>
   </si>
   <si>
@@ -260,9 +257,6 @@
     <t>R29</t>
   </si>
   <si>
-    <t>R31</t>
-  </si>
-  <si>
     <t>100k</t>
   </si>
   <si>
@@ -440,9 +434,6 @@
     <t>aan stijn vragen</t>
   </si>
   <si>
-    <t>nog zoeken</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.mouser.be/ProductDetail/Murata-Electronics/LQM21DH150M70L?qs=W%2FMpXkg%252BdQ4Uesp%252BQGOKoQ%3D%3D </t>
   </si>
   <si>
@@ -513,6 +504,36 @@
   </si>
   <si>
     <t>https://www.mouser.be/ProductDetail/Bulgin/C1353ATNAN?qs=T3oQrply3y900zDyRgtbfw%3D%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.mouser.be/ProductDetail/TDK/TFM322512ALMA1R5MTAA?qs=BJlw7L4Cy7%252BBL%2F0%252BEKaU4A%3D%3D </t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/TDK/SPM10065VT-2R2M-D?qs=vmHwEFxEFR9gnE%252BaAfMtAw%3D%3D</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Panasonic/EEH-ZF1V101P?qs=sGAEpiMZZMvwFf0viD3Y3a3yb5D6sPUgUc143nXe4dHlPMZUEzhyaQ%3D%3D</t>
+  </si>
+  <si>
+    <t>R1, R3,  R4, R6, R7, R10, R11, R13, R16, R20, R22, R28, R32, R37</t>
+  </si>
+  <si>
+    <t>R5, R8, R9, R31</t>
+  </si>
+  <si>
+    <t>D26</t>
+  </si>
+  <si>
+    <t>1,8V</t>
+  </si>
+  <si>
+    <t>Zener Diode</t>
+  </si>
+  <si>
+    <t>zener diode</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/ON-Semiconductor/MMSZ4678T1G?qs=P4IOph%252Bbot8vK8FZ3ltvyA%3D%3D</t>
   </si>
 </sst>
 </file>
@@ -872,10 +893,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F6" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G33" sqref="G33"/>
+    <sheetView tabSelected="1" topLeftCell="F19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -932,7 +953,7 @@
         <v>9</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="18" x14ac:dyDescent="0.35">
@@ -975,11 +996,13 @@
       <c r="F4" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="2"/>
+      <c r="G4" s="6" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="5" spans="1:7" ht="126" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B5" s="4">
         <v>31</v>
@@ -997,12 +1020,12 @@
         <v>9</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="36" x14ac:dyDescent="0.35">
       <c r="A6" s="4" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B6" s="4">
         <v>5</v>
@@ -1020,7 +1043,7 @@
         <v>9</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="18" x14ac:dyDescent="0.35">
@@ -1043,12 +1066,12 @@
         <v>9</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A8" s="4" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="B8" s="4">
         <v>2</v>
@@ -1066,7 +1089,7 @@
         <v>9</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="36" x14ac:dyDescent="0.35">
@@ -1089,7 +1112,7 @@
         <v>9</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="18" x14ac:dyDescent="0.35">
@@ -1112,7 +1135,7 @@
         <v>9</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="18" x14ac:dyDescent="0.35">
@@ -1135,7 +1158,7 @@
         <v>9</v>
       </c>
       <c r="G11" s="6" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="18" x14ac:dyDescent="0.35">
@@ -1158,7 +1181,7 @@
         <v>9</v>
       </c>
       <c r="G12" s="6" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="18" x14ac:dyDescent="0.35">
@@ -1181,7 +1204,7 @@
         <v>36</v>
       </c>
       <c r="G13" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="90" x14ac:dyDescent="0.35">
@@ -1204,7 +1227,7 @@
         <v>41</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="72" x14ac:dyDescent="0.35">
@@ -1227,7 +1250,7 @@
         <v>45</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>160</v>
+        <v>157</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="18" x14ac:dyDescent="0.35">
@@ -1250,7 +1273,7 @@
         <v>49</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="72" x14ac:dyDescent="0.35">
@@ -1269,7 +1292,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="2" t="s">
-        <v>161</v>
+        <v>158</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="18" x14ac:dyDescent="0.35">
@@ -1292,7 +1315,7 @@
         <v>56</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="18" x14ac:dyDescent="0.35">
@@ -1314,8 +1337,8 @@
       <c r="F19" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>138</v>
+      <c r="G19" s="6" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="18" x14ac:dyDescent="0.35">
@@ -1337,8 +1360,8 @@
       <c r="F20" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>138</v>
+      <c r="G20" s="6" t="s">
+        <v>161</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="18" x14ac:dyDescent="0.35">
@@ -1361,35 +1384,35 @@
         <v>64</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="54" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B22" s="4">
+        <v>14</v>
+      </c>
+      <c r="C22" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="B22" s="4">
-        <v>12</v>
-      </c>
-      <c r="C22" s="4" t="s">
+      <c r="D22" s="4" t="s">
         <v>66</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="E22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E22" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="G22" s="6" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A23" s="4" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B23" s="4">
         <v>1</v>
@@ -1398,21 +1421,21 @@
         <v>100</v>
       </c>
       <c r="D23" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F23" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E23" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="G23" s="6" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A24" s="4" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B24" s="4">
         <v>1</v>
@@ -1421,90 +1444,90 @@
         <v>560</v>
       </c>
       <c r="D24" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F24" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E24" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="G24" s="6" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A25" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B25" s="4">
+        <v>1</v>
+      </c>
+      <c r="C25" s="4" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="4">
-        <v>1</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>72</v>
-      </c>
       <c r="D25" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F25" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E25" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="G25" s="6" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A26" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B26" s="4">
         <v>4</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D26" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F26" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E26" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="G26" s="6" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B27" s="4">
         <v>2</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D27" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F27" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E27" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F27" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="G27" s="6" t="s">
-        <v>146</v>
+        <v>143</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A28" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B28" s="4">
         <v>1</v>
@@ -1513,287 +1536,310 @@
         <v>10</v>
       </c>
       <c r="D28" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E28" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E28" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>68</v>
-      </c>
       <c r="G28" s="6" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
-        <v>78</v>
+        <v>165</v>
       </c>
       <c r="B29" s="4">
         <v>1</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>79</v>
+        <v>166</v>
       </c>
       <c r="D29" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="E29" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="4" t="s">
+        <v>168</v>
+      </c>
+      <c r="G29" s="6" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" ht="18" x14ac:dyDescent="0.35">
+      <c r="A30" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B30" s="4">
+        <v>4</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>77</v>
+      </c>
+      <c r="D30" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="E30" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F30" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="E29" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" ht="36" x14ac:dyDescent="0.35">
-      <c r="A30" s="4" t="s">
-        <v>80</v>
-      </c>
-      <c r="B30" s="4">
-        <v>6</v>
-      </c>
-      <c r="C30" s="4" t="s">
-        <v>81</v>
-      </c>
-      <c r="D30" s="4" t="s">
-        <v>82</v>
-      </c>
-      <c r="E30" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F30" s="4" t="s">
-        <v>83</v>
-      </c>
       <c r="G30" s="6" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="36" x14ac:dyDescent="0.35">
       <c r="A31" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B31" s="4">
+        <v>6</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="D31" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="E31" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F31" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G31" s="6" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" ht="36" x14ac:dyDescent="0.35">
+      <c r="A32" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="B32" s="4">
+        <v>1</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="D32" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="B31" s="4">
-        <v>1</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>85</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="6" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A32" s="4" t="s">
-        <v>87</v>
-      </c>
-      <c r="B32" s="4">
-        <v>1</v>
-      </c>
-      <c r="C32" s="4" t="s">
-        <v>88</v>
-      </c>
-      <c r="D32" s="4" t="s">
-        <v>89</v>
       </c>
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="6" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" ht="54" x14ac:dyDescent="0.35">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A33" s="4" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B33" s="4">
         <v>1</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
-      <c r="G33" s="2" t="s">
-        <v>140</v>
+      <c r="G33" s="6" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="54" x14ac:dyDescent="0.35">
       <c r="A34" s="4" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="B34" s="4">
         <v>1</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E34" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="F34" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="G34" s="6" t="s">
-        <v>151</v>
+        <v>90</v>
+      </c>
+      <c r="E34" s="4"/>
+      <c r="F34" s="4"/>
+      <c r="G34" s="2" t="s">
+        <v>137</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="54" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
       <c r="B35" s="4">
         <v>1</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>100</v>
+        <v>93</v>
       </c>
       <c r="E35" s="4" t="s">
-        <v>101</v>
+        <v>94</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="54" x14ac:dyDescent="0.35">
       <c r="A36" s="4" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="B36" s="4">
         <v>1</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="D36" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="2" t="s">
-        <v>153</v>
+        <v>98</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="F36" s="4" t="s">
+        <v>100</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="54" x14ac:dyDescent="0.35">
       <c r="A37" s="4" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="B37" s="4">
         <v>1</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D37" s="4" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
-      <c r="G37" s="6" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" ht="72" x14ac:dyDescent="0.35">
+      <c r="G37" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" ht="54" x14ac:dyDescent="0.35">
       <c r="A38" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B38" s="4">
+        <v>1</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="D38" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="E38" s="4"/>
+      <c r="F38" s="4"/>
+      <c r="G38" s="6" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" ht="72" x14ac:dyDescent="0.35">
+      <c r="A39" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B39" s="4">
+        <v>1</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D39" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="B38" s="4">
-        <v>1</v>
-      </c>
-      <c r="C38" s="4" t="s">
+      <c r="E39" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="F39" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="G39" s="6" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="40" spans="1:7" ht="36" x14ac:dyDescent="0.35">
+      <c r="A40" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="F38" s="4" t="s">
+      <c r="B40" s="4">
+        <v>1</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="G38" s="6" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" ht="36" x14ac:dyDescent="0.35">
-      <c r="A39" s="4" t="s">
+      <c r="D40" s="4" t="s">
         <v>114</v>
-      </c>
-      <c r="B39" s="4">
-        <v>1</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="6" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="40" spans="1:7" ht="18" x14ac:dyDescent="0.35">
-      <c r="A40" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="B40" s="4">
-        <v>1</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>119</v>
       </c>
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="6" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="41" spans="1:7" ht="72" x14ac:dyDescent="0.35">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="41" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A41" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="B41" s="4">
+        <v>1</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="D41" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="E41" s="4"/>
+      <c r="F41" s="4"/>
+      <c r="G41" s="6" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="42" spans="1:7" ht="72" x14ac:dyDescent="0.35">
+      <c r="A42" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="B42" s="4">
+        <v>1</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="D42" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="B41" s="4">
-        <v>1</v>
-      </c>
-      <c r="C41" s="4" t="s">
+      <c r="E42" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="D41" s="4" t="s">
+      <c r="F42" s="4" t="s">
         <v>122</v>
       </c>
-      <c r="E41" s="4" t="s">
-        <v>123</v>
-      </c>
-      <c r="F41" s="4" t="s">
-        <v>124</v>
-      </c>
-      <c r="G41" s="7" t="s">
-        <v>158</v>
+      <c r="G42" s="7" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>
@@ -1815,21 +1861,24 @@
     <hyperlink ref="G26" r:id="rId15"/>
     <hyperlink ref="G27" r:id="rId16"/>
     <hyperlink ref="G28" r:id="rId17"/>
-    <hyperlink ref="G29" r:id="rId18"/>
-    <hyperlink ref="G30" r:id="rId19"/>
-    <hyperlink ref="G32" r:id="rId20"/>
-    <hyperlink ref="G34" r:id="rId21"/>
-    <hyperlink ref="G35" r:id="rId22"/>
-    <hyperlink ref="G37" r:id="rId23"/>
-    <hyperlink ref="G38" r:id="rId24"/>
-    <hyperlink ref="G39" r:id="rId25"/>
-    <hyperlink ref="G40" r:id="rId26"/>
-    <hyperlink ref="G41" r:id="rId27"/>
+    <hyperlink ref="G30" r:id="rId18"/>
+    <hyperlink ref="G31" r:id="rId19"/>
+    <hyperlink ref="G33" r:id="rId20"/>
+    <hyperlink ref="G35" r:id="rId21"/>
+    <hyperlink ref="G36" r:id="rId22"/>
+    <hyperlink ref="G38" r:id="rId23"/>
+    <hyperlink ref="G39" r:id="rId24"/>
+    <hyperlink ref="G40" r:id="rId25"/>
+    <hyperlink ref="G41" r:id="rId26"/>
+    <hyperlink ref="G42" r:id="rId27"/>
     <hyperlink ref="G16" r:id="rId28"/>
     <hyperlink ref="G15" r:id="rId29"/>
-    <hyperlink ref="G31" r:id="rId30"/>
+    <hyperlink ref="G32" r:id="rId30"/>
+    <hyperlink ref="G19" r:id="rId31"/>
+    <hyperlink ref="G20" r:id="rId32"/>
+    <hyperlink ref="G4" r:id="rId33"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId31"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId34"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
aanpassingen bom, gerber files voor bestelling
</commit_message>
<xml_diff>
--- a/Bluetooth music box/schema's en pcb/schema_v1/BOM.xlsx
+++ b/Bluetooth music box/schema's en pcb/schema_v1/BOM.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="177">
   <si>
     <t>Ref</t>
   </si>
@@ -431,9 +431,6 @@
     <t>Heb ik zelf</t>
   </si>
   <si>
-    <t>aan stijn vragen</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.mouser.be/ProductDetail/Murata-Electronics/LQM21DH150M70L?qs=W%2FMpXkg%252BdQ4Uesp%252BQGOKoQ%3D%3D </t>
   </si>
   <si>
@@ -491,9 +488,6 @@
     <t>https://www.mouser.be/ProductDetail/Analog-Devices/LTC4001EUFPBF?qs=hVkxg5c3xu8HPrD%252BhnhkYg%3D%3D</t>
   </si>
   <si>
-    <t>https://www.mouser.be/ProductDetail/Texas-Instruments/TPS563200DDCR?qs=bT6MOr62zwLjxJIF4PA64g%3D%3D</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://www.mouser.be/ProductDetail/Wurth-Elektronik/629105136821?qs=P%2FTEqz%252BQfncvaTjfhhJgDA%3D%3D </t>
   </si>
   <si>
@@ -533,7 +527,34 @@
     <t>zener diode</t>
   </si>
   <si>
-    <t>https://www.mouser.be/ProductDetail/ON-Semiconductor/MMSZ4678T1G?qs=P4IOph%252Bbot8vK8FZ3ltvyA%3D%3D</t>
+    <t>aan stijn vragen (in orde)</t>
+  </si>
+  <si>
+    <t>https://www.mouser.be/ProductDetail/Comchip-Technology/MMSZ4678-HF?qs=GBLSl2AkirsCXt3Ql7prKg%3D%3D</t>
+  </si>
+  <si>
+    <t>https://sinuss.be/componenten/halfgeleiders-sensors/ics/voltage-regulators/dc-dc-switching-regulators-adjustable/2450170-tps563200ddct-dcdc-conv-sync-buck-650khz-sot-23-6-texas-instruments</t>
+  </si>
+  <si>
+    <t>Bestelling</t>
+  </si>
+  <si>
+    <t>sinuss</t>
+  </si>
+  <si>
+    <t>pcb</t>
+  </si>
+  <si>
+    <t>mouser</t>
+  </si>
+  <si>
+    <t>aliexpress</t>
+  </si>
+  <si>
+    <t>besteld</t>
+  </si>
+  <si>
+    <t>totaal</t>
   </si>
 </sst>
 </file>
@@ -893,10 +914,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G42"/>
+  <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F19" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" topLeftCell="A37" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B53" sqref="B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -997,7 +1018,7 @@
         <v>20</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="126" x14ac:dyDescent="0.35">
@@ -1227,7 +1248,7 @@
         <v>41</v>
       </c>
       <c r="G14" s="2" t="s">
-        <v>135</v>
+        <v>167</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="72" x14ac:dyDescent="0.35">
@@ -1250,7 +1271,7 @@
         <v>45</v>
       </c>
       <c r="G15" s="6" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="18" x14ac:dyDescent="0.35">
@@ -1273,7 +1294,7 @@
         <v>49</v>
       </c>
       <c r="G16" s="6" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="72" x14ac:dyDescent="0.35">
@@ -1292,7 +1313,7 @@
       <c r="E17" s="4"/>
       <c r="F17" s="4"/>
       <c r="G17" s="2" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="18" x14ac:dyDescent="0.35">
@@ -1315,7 +1336,7 @@
         <v>56</v>
       </c>
       <c r="G18" s="6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="18" x14ac:dyDescent="0.35">
@@ -1338,7 +1359,7 @@
         <v>56</v>
       </c>
       <c r="G19" s="6" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="18" x14ac:dyDescent="0.35">
@@ -1361,7 +1382,7 @@
         <v>56</v>
       </c>
       <c r="G20" s="6" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="18" x14ac:dyDescent="0.35">
@@ -1384,12 +1405,12 @@
         <v>64</v>
       </c>
       <c r="G21" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="54" x14ac:dyDescent="0.35">
       <c r="A22" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="B22" s="4">
         <v>14</v>
@@ -1407,7 +1428,7 @@
         <v>67</v>
       </c>
       <c r="G22" s="6" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="18" x14ac:dyDescent="0.35">
@@ -1430,7 +1451,7 @@
         <v>67</v>
       </c>
       <c r="G23" s="6" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="18" x14ac:dyDescent="0.35">
@@ -1453,7 +1474,7 @@
         <v>67</v>
       </c>
       <c r="G24" s="6" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="18" x14ac:dyDescent="0.35">
@@ -1476,7 +1497,7 @@
         <v>67</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="18" x14ac:dyDescent="0.35">
@@ -1499,7 +1520,7 @@
         <v>67</v>
       </c>
       <c r="G26" s="6" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="18" x14ac:dyDescent="0.35">
@@ -1522,7 +1543,7 @@
         <v>67</v>
       </c>
       <c r="G27" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="18" x14ac:dyDescent="0.35">
@@ -1545,35 +1566,35 @@
         <v>67</v>
       </c>
       <c r="G28" s="6" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A29" s="4" t="s">
+        <v>163</v>
+      </c>
+      <c r="B29" s="4">
+        <v>1</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="D29" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B29" s="4">
-        <v>1</v>
-      </c>
-      <c r="C29" s="4" t="s">
+      <c r="E29" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F29" s="4" t="s">
         <v>166</v>
       </c>
-      <c r="D29" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="E29" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="F29" s="4" t="s">
+      <c r="G29" s="6" t="s">
         <v>168</v>
-      </c>
-      <c r="G29" s="6" t="s">
-        <v>169</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="18" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B30" s="4">
         <v>4</v>
@@ -1591,7 +1612,7 @@
         <v>67</v>
       </c>
       <c r="G30" s="6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="36" x14ac:dyDescent="0.35">
@@ -1614,7 +1635,7 @@
         <v>81</v>
       </c>
       <c r="G31" s="6" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="32" spans="1:7" ht="36" x14ac:dyDescent="0.35">
@@ -1633,7 +1654,7 @@
       <c r="E32" s="4"/>
       <c r="F32" s="4"/>
       <c r="G32" s="6" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="33" spans="1:7" ht="18" x14ac:dyDescent="0.35">
@@ -1652,7 +1673,7 @@
       <c r="E33" s="4"/>
       <c r="F33" s="4"/>
       <c r="G33" s="6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="34" spans="1:7" ht="54" x14ac:dyDescent="0.35">
@@ -1671,7 +1692,7 @@
       <c r="E34" s="4"/>
       <c r="F34" s="4"/>
       <c r="G34" s="2" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="54" x14ac:dyDescent="0.35">
@@ -1694,7 +1715,7 @@
         <v>95</v>
       </c>
       <c r="G35" s="6" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="36" spans="1:7" ht="54" x14ac:dyDescent="0.35">
@@ -1717,7 +1738,7 @@
         <v>100</v>
       </c>
       <c r="G36" s="6" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="37" spans="1:7" ht="54" x14ac:dyDescent="0.35">
@@ -1736,7 +1757,7 @@
       <c r="E37" s="4"/>
       <c r="F37" s="4"/>
       <c r="G37" s="2" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="38" spans="1:7" ht="54" x14ac:dyDescent="0.35">
@@ -1755,7 +1776,7 @@
       <c r="E38" s="4"/>
       <c r="F38" s="4"/>
       <c r="G38" s="6" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="39" spans="1:7" ht="72" x14ac:dyDescent="0.35">
@@ -1778,7 +1799,7 @@
         <v>111</v>
       </c>
       <c r="G39" s="6" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="40" spans="1:7" ht="36" x14ac:dyDescent="0.35">
@@ -1797,7 +1818,7 @@
       <c r="E40" s="4"/>
       <c r="F40" s="4"/>
       <c r="G40" s="6" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="18" x14ac:dyDescent="0.35">
@@ -1816,7 +1837,7 @@
       <c r="E41" s="4"/>
       <c r="F41" s="4"/>
       <c r="G41" s="6" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="42" spans="1:7" ht="72" x14ac:dyDescent="0.35">
@@ -1839,7 +1860,65 @@
         <v>122</v>
       </c>
       <c r="G42" s="7" t="s">
-        <v>155</v>
+        <v>169</v>
+      </c>
+    </row>
+    <row r="46" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A46" s="5" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="47" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A47" s="5" t="s">
+        <v>171</v>
+      </c>
+      <c r="B47" s="5">
+        <v>10.49</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A48" s="5" t="s">
+        <v>172</v>
+      </c>
+      <c r="B48" s="5">
+        <v>56.85</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A49" s="5" t="s">
+        <v>173</v>
+      </c>
+      <c r="B49" s="5">
+        <v>139.82</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A50" s="5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B50" s="5">
+        <v>11.3</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A52" s="5" t="s">
+        <v>176</v>
+      </c>
+      <c r="B52" s="5">
+        <f>B47+B48+B49+B50</f>
+        <v>218.46</v>
       </c>
     </row>
   </sheetData>
@@ -1877,8 +1956,9 @@
     <hyperlink ref="G19" r:id="rId31"/>
     <hyperlink ref="G20" r:id="rId32"/>
     <hyperlink ref="G4" r:id="rId33"/>
+    <hyperlink ref="G29" r:id="rId34"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId34"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId35"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Werken aan positionering componenten op pcb
kleine aanpassingen op schema (zoals verbinding leds - µc)
</commit_message>
<xml_diff>
--- a/Bluetooth music box/schema's en pcb/schema_v1/BOM.xlsx
+++ b/Bluetooth music box/schema's en pcb/schema_v1/BOM.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2364" windowHeight="0"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -916,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F31" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G33" activeCellId="1" sqref="C33 G33"/>
+    <sheetView tabSelected="1" topLeftCell="F14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G15" activeCellId="1" sqref="C5 G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Tracks tekenen op pcb
</commit_message>
<xml_diff>
--- a/Bluetooth music box/schema's en pcb/schema_v1/BOM.xlsx
+++ b/Bluetooth music box/schema's en pcb/schema_v1/BOM.xlsx
@@ -916,8 +916,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F14" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G15" activeCellId="1" sqref="C5 G15"/>
+    <sheetView tabSelected="1" topLeftCell="F35" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G41" activeCellId="4" sqref="C5 G15 G36 G39 G41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>